<commit_message>
Updates will beneficiary location roll up
</commit_message>
<xml_diff>
--- a/schema/summary-table/360-giving-schema-titles.xlsx
+++ b/schema/summary-table/360-giving-schema-titles.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>Identifier</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Beneficiary Location:Country Code</t>
+  </si>
+  <si>
+    <t>Beneficiary Location:Latitude</t>
+  </si>
+  <si>
+    <t>Beneficiary Location:Longitude</t>
+  </si>
+  <si>
+    <t>Beneficiary Location:Geographic Code</t>
+  </si>
+  <si>
+    <t>Beneficiary Location:Geographic Code Type</t>
   </si>
   <si>
     <t>Funding Org:Identifier</t>
@@ -594,7 +606,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,7 +614,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,6 +710,18 @@
       </c>
       <c r="AF1" t="s">
         <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -720,19 +744,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -741,10 +765,10 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -767,10 +791,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -785,10 +809,10 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -811,34 +835,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -861,13 +885,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -876,10 +900,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -902,46 +926,46 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -964,64 +988,64 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="Q1" t="s">
         <v>2</v>
       </c>
       <c r="R1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="S1" t="s">
         <v>3</v>
       </c>
       <c r="T1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1044,43 +1068,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update flatten-tool to fix org location title headings in template
OpenDataServices/flatten-tool#100
</commit_message>
<xml_diff>
--- a/schema/summary-table/360-giving-schema-titles.xlsx
+++ b/schema/summary-table/360-giving-schema-titles.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>Identifier</t>
   </si>
@@ -195,31 +195,31 @@
     <t>fundingOrganization/0/Identifier</t>
   </si>
   <si>
-    <t>Location:Identifier</t>
-  </si>
-  <si>
-    <t>Location:Name</t>
-  </si>
-  <si>
-    <t>Location:Country Code</t>
-  </si>
-  <si>
-    <t>Location:Latitude</t>
-  </si>
-  <si>
-    <t>Location:Longitude</t>
-  </si>
-  <si>
-    <t>Location:Description</t>
-  </si>
-  <si>
-    <t>Location:Geographic Code</t>
-  </si>
-  <si>
-    <t>Location:Geographic Code Type</t>
-  </si>
-  <si>
-    <t>Location:Last modified</t>
+    <t>Funding Org:Location:Identifier</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Name</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Country Code</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Latitude</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Longitude</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Description</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Geographic Code</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Geographic Code Type</t>
+  </si>
+  <si>
+    <t>Funding Org:Location:Last modified</t>
   </si>
   <si>
     <t>Funding Org:Contact Name</t>
@@ -301,6 +301,33 @@
   </si>
   <si>
     <t>recipientOrganization/0/Identifier</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Identifier</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Name</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Country Code</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Latitude</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Longitude</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Description</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Geographic Code</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Geographic Code Type</t>
+  </si>
+  <si>
+    <t>Recipient Org:Location:Last modified</t>
   </si>
   <si>
     <t>Recipient Org:Department</t>
@@ -953,31 +980,31 @@
         <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1010,10 +1037,10 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -1037,25 +1064,25 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="N1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="O1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="P1" t="s">
         <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1082,22 +1109,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build new summary reference tables using flatten-tool
</commit_message>
<xml_diff>
--- a/schema/summary-table/360-giving-schema-titles.xlsx
+++ b/schema/summary-table/360-giving-schema-titles.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>Identifier</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Classifications:Last modified</t>
   </si>
   <si>
-    <t>fundingOrganization/0/Identifier</t>
-  </si>
-  <si>
     <t>Funding Org:Location:Identifier</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
   </si>
   <si>
     <t>Planned Dates:Last modified</t>
-  </si>
-  <si>
-    <t>recipientOrganization/0/Identifier</t>
   </si>
   <si>
     <t>Recipient Org:Location:Identifier</t>
@@ -854,22 +848,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -902,13 +896,13 @@
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -947,10 +941,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
         <v>88</v>
-      </c>
-      <c r="G1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -977,34 +971,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>97</v>
-      </c>
-      <c r="J1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K1" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1037,10 +1031,10 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -1064,25 +1058,25 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" t="s">
         <v>102</v>
-      </c>
-      <c r="N1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" t="s">
-        <v>104</v>
       </c>
       <c r="P1" t="s">
         <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1109,22 +1103,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>110</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1358,34 +1352,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
-      </c>
-      <c r="K1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1421,49 +1415,49 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>74</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>77</v>
-      </c>
-      <c r="S1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>